<commit_message>
add export file in output
</commit_message>
<xml_diff>
--- a/outputs/VaraintBasedArray.xlsx
+++ b/outputs/VaraintBasedArray.xlsx
@@ -13093,7 +13093,7 @@
         </is>
       </c>
       <c r="M201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202">
@@ -13156,7 +13156,7 @@
         </is>
       </c>
       <c r="M202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203">
@@ -13219,7 +13219,7 @@
         </is>
       </c>
       <c r="M203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204">
@@ -13282,7 +13282,7 @@
         </is>
       </c>
       <c r="M204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205">
@@ -13345,7 +13345,7 @@
         </is>
       </c>
       <c r="M205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206">
@@ -13408,7 +13408,7 @@
         </is>
       </c>
       <c r="M206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207">
@@ -13471,7 +13471,7 @@
         </is>
       </c>
       <c r="M207" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208">
@@ -13534,7 +13534,7 @@
         </is>
       </c>
       <c r="M208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209">
@@ -13597,7 +13597,7 @@
         </is>
       </c>
       <c r="M209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210">
@@ -13660,7 +13660,7 @@
         </is>
       </c>
       <c r="M210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211">
@@ -13723,7 +13723,7 @@
         </is>
       </c>
       <c r="M211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212">
@@ -13786,7 +13786,7 @@
         </is>
       </c>
       <c r="M212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213">
@@ -13849,7 +13849,7 @@
         </is>
       </c>
       <c r="M213" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="214">
@@ -13912,7 +13912,7 @@
         </is>
       </c>
       <c r="M214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215">
@@ -13975,7 +13975,7 @@
         </is>
       </c>
       <c r="M215" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216">
@@ -14038,7 +14038,7 @@
         </is>
       </c>
       <c r="M216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217">
@@ -14101,7 +14101,7 @@
         </is>
       </c>
       <c r="M217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218">
@@ -14164,7 +14164,7 @@
         </is>
       </c>
       <c r="M218" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219">
@@ -14227,7 +14227,7 @@
         </is>
       </c>
       <c r="M219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220">
@@ -14290,7 +14290,7 @@
         </is>
       </c>
       <c r="M220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221">
@@ -14353,7 +14353,7 @@
         </is>
       </c>
       <c r="M221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222">
@@ -14416,7 +14416,7 @@
         </is>
       </c>
       <c r="M222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223">
@@ -14479,7 +14479,7 @@
         </is>
       </c>
       <c r="M223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224">
@@ -14542,7 +14542,7 @@
         </is>
       </c>
       <c r="M224" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225">
@@ -14605,7 +14605,7 @@
         </is>
       </c>
       <c r="M225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226">
@@ -14668,7 +14668,7 @@
         </is>
       </c>
       <c r="M226" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227">
@@ -14731,7 +14731,7 @@
         </is>
       </c>
       <c r="M227" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228">
@@ -14794,7 +14794,7 @@
         </is>
       </c>
       <c r="M228" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229">
@@ -14857,7 +14857,7 @@
         </is>
       </c>
       <c r="M229" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230">
@@ -14920,7 +14920,7 @@
         </is>
       </c>
       <c r="M230" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="231">
@@ -14983,7 +14983,7 @@
         </is>
       </c>
       <c r="M231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232">
@@ -15046,7 +15046,7 @@
         </is>
       </c>
       <c r="M232" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233">
@@ -15109,7 +15109,7 @@
         </is>
       </c>
       <c r="M233" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="234">
@@ -15172,7 +15172,7 @@
         </is>
       </c>
       <c r="M234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235">
@@ -15235,7 +15235,7 @@
         </is>
       </c>
       <c r="M235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236">
@@ -15298,7 +15298,7 @@
         </is>
       </c>
       <c r="M236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237">
@@ -15361,7 +15361,7 @@
         </is>
       </c>
       <c r="M237" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238">
@@ -15424,7 +15424,7 @@
         </is>
       </c>
       <c r="M238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239">
@@ -15487,7 +15487,7 @@
         </is>
       </c>
       <c r="M239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="240">
@@ -15550,7 +15550,7 @@
         </is>
       </c>
       <c r="M240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="241">
@@ -15613,7 +15613,7 @@
         </is>
       </c>
       <c r="M241" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="242">
@@ -15676,7 +15676,7 @@
         </is>
       </c>
       <c r="M242" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243">
@@ -15739,7 +15739,7 @@
         </is>
       </c>
       <c r="M243" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="244">
@@ -15802,7 +15802,7 @@
         </is>
       </c>
       <c r="M244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>